<commit_message>
almost done with correct parsing form deepgtav to yolo format
</commit_message>
<xml_diff>
--- a/VPilot/visualization/Decision on the classes.xlsx
+++ b/VPilot/visualization/Decision on the classes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t xml:space="preserve">Vanilla</t>
   </si>
@@ -121,6 +121,31 @@
     <t xml:space="preserve">others</t>
   </si>
   <si>
+    <t xml:space="preserve">Boats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Railed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Names found in the Data generated for Khalil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Airplane',
+ 'Animal',
+ 'Boat',
+ 'Bus',
+ 'Car',
+ 'Cyclist',
+ 'Motorbike',
+ 'Pedestrian',
+ 'Person_sitting',
+ 'Railed',
+ 'Trailer',
+ 'Truck',
+ 'Utility'}
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Combined Order</t>
   </si>
   <si>
@@ -133,10 +158,13 @@
     <t xml:space="preserve">Class Number</t>
   </si>
   <si>
+    <t xml:space="preserve">New Class Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">REMOVED</t>
   </si>
   <si>
-    <t xml:space="preserve">Maybe i can also get people on vehicles</t>
+    <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">Also look for car models</t>
@@ -230,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +269,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,13 +292,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.01"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -417,221 +452,281 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="167.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>13</v>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I30" s="0" t="n">
+      <c r="G35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="1" t="s">
-        <v>41</v>
+      <c r="A39" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="0" t="n">
+      <c r="I45" s="1" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="1" t="s">
+      <c r="K45" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I41" s="0" t="n">
+      <c r="G46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="1" t="n">
         <v>11</v>
       </c>
     </row>

</xml_diff>